<commit_message>
scrape enhance and rl training v0.1
</commit_message>
<xml_diff>
--- a/asset_ticker_list.xlsx
+++ b/asset_ticker_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pythonfiles\FinNLP7036\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4E85A8-2F94-4905-9195-68CA8740AEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632419BD-F63E-47C7-AADA-9AC80F261BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="18612" windowHeight="10236" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>StockTwits_code</t>
   </si>
@@ -78,27 +78,42 @@
     <t>SPX</t>
   </si>
   <si>
+    <t>FTSE</t>
+  </si>
+  <si>
+    <t>CAC40</t>
+  </si>
+  <si>
+    <t>STOXX</t>
+  </si>
+  <si>
+    <t>SENSEX</t>
+  </si>
+  <si>
+    <t>SSEC</t>
+  </si>
+  <si>
+    <t>NIFTY50.NSE</t>
+  </si>
+  <si>
+    <t>HSCEI</t>
+  </si>
+  <si>
+    <t>SLV</t>
+  </si>
+  <si>
+    <t>GLD</t>
+  </si>
+  <si>
+    <t>USO</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
     <t>DJI</t>
   </si>
   <si>
-    <t>FTSE</t>
-  </si>
-  <si>
-    <t>CAC40</t>
-  </si>
-  <si>
-    <t>STOXX</t>
-  </si>
-  <si>
-    <t>SENSEX</t>
-  </si>
-  <si>
-    <t>SSEC</t>
-  </si>
-  <si>
-    <t>NIFTY50.NSE</t>
-  </si>
-  <si>
     <t>GOLD</t>
   </si>
   <si>
@@ -108,19 +123,29 @@
     <t>OIL</t>
   </si>
   <si>
-    <t>HSCEI</t>
+    <t>IXIC</t>
+  </si>
+  <si>
+    <t>GSPC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -274,38 +299,41 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -575,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A13" sqref="A13:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -587,122 +615,140 @@
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" ht="15" thickBot="1">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="B13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1">
+      <c r="B14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="11" t="s">
         <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>